<commit_message>
03_Sprint_Backlogs.xlsx: Aktualisiert, aber noch nicht auf Stand!
</commit_message>
<xml_diff>
--- a/1. Projektplanung/03_Sprint_Backlogs.xlsx
+++ b/1. Projektplanung/03_Sprint_Backlogs.xlsx
@@ -1,13 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://thude0-my.sharepoint.com/personal/jecklu01_hs-ulm_de/Documents/5. Semester/Software Projekt/RaytRazor/1. Projektplanung/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="197" documentId="11_AD4DB114E441178AC67DF4622615E776693EDF11" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DDBF27A5-4643-488B-9C4F-9F2C570D61B7}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sprint 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sprint 2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sprint 3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sprint 4" sheetId="4" r:id="rId4"/>
+    <sheet name="Sprint 5" sheetId="5" r:id="rId5"/>
+    <sheet name="Sprint 6" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -18,9 +29,119 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="35">
+  <si>
+    <t>Aufgabe</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>JSON Szenen Export</t>
+  </si>
+  <si>
+    <t>abgeschlossen</t>
+  </si>
+  <si>
+    <t>Raytracing verbessern (OpenMP)</t>
+  </si>
+  <si>
+    <t>noch offen</t>
+  </si>
+  <si>
+    <t>SzeneManager  implementieren</t>
+  </si>
+  <si>
+    <t>Error-Handling durch logging via Logger verbessern</t>
+  </si>
+  <si>
+    <t>3D-Preview -&gt; mehrere Objekte darstellen</t>
+  </si>
+  <si>
+    <t>in arbeit</t>
+  </si>
+  <si>
+    <t>3D-Preview -&gt; Lichtquellen</t>
+  </si>
+  <si>
+    <t>3D-Preview -&gt; Objekte anzeigen aus JSON import</t>
+  </si>
+  <si>
+    <t>Json Szenen Import Segmentation Errors beheben</t>
+  </si>
+  <si>
+    <t>Raytracing Bild export implementieren</t>
+  </si>
+  <si>
+    <t>Backend-Aufgaben</t>
+  </si>
+  <si>
+    <t>Frontend-Aufgaben</t>
+  </si>
+  <si>
+    <t>UI-Verschönern</t>
+  </si>
+  <si>
+    <t>Dynamische Größenanpassbarkeit ermöglichen</t>
+  </si>
+  <si>
+    <t>Raytracing (SDL) in NanoGUI Fenster mit einbinden</t>
+  </si>
+  <si>
+    <t>Kritikalität</t>
+  </si>
+  <si>
+    <t>hoch</t>
+  </si>
+  <si>
+    <t>3D-Preview -&gt; übergabe an Raytracer</t>
+  </si>
+  <si>
+    <t>medium</t>
+  </si>
+  <si>
+    <t>Übersicht über verschiedene Raytracing Arten verschaffen</t>
+  </si>
+  <si>
+    <t>Übersicht über math. Formeln für Raytracing verschaffen</t>
+  </si>
+  <si>
+    <t>Eigene Mathe-Bibliothek für Raytracing schreiben</t>
+  </si>
+  <si>
+    <t>abgebrochen</t>
+  </si>
+  <si>
+    <t>GitHub Commit Layout definieren</t>
+  </si>
+  <si>
+    <t>GitHub Repository erstellen</t>
+  </si>
+  <si>
+    <t>Visionspräsentation erstellen und Präsentation abhalten</t>
+  </si>
+  <si>
+    <t>Team Zusammenstellung Hr. Lunde mitteilen</t>
+  </si>
+  <si>
+    <t>Mit .obj und .mtl Formaten vertraut machen</t>
+  </si>
+  <si>
+    <t>Allgemeine Aufgaben</t>
+  </si>
+  <si>
+    <t>Frontend Aufgaben</t>
+  </si>
+  <si>
+    <t>Backend Aufgaben</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -28,16 +149,54 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -45,15 +204,38 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -66,6 +248,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -330,13 +516,815 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="50.7109375" customWidth="1"/>
+    <col min="2" max="3" width="15.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="2"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="2"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="2"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="2"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="2"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="2"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="2"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="2"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="2"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="2"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="2"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A12:C12"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F604C2F-B85D-43C9-892C-B1D90A990BEC}">
+  <dimension ref="A1:C16"/>
+  <sheetViews>
+    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="50.7109375" customWidth="1"/>
+    <col min="2" max="3" width="15.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="2"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="2"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="2"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="2"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="2"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="2"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="2"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="2"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="2"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="2"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="2"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A13:C13"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F033D8F3-60F5-4555-AEA9-6349E4C0E2BD}">
+  <dimension ref="A1:C16"/>
+  <sheetViews>
+    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="50.7109375" customWidth="1"/>
+    <col min="2" max="3" width="15.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="2"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="2"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="2"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="2"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="2"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="2"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="2"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="2"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="2"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="2"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="2"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A13:C13"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC71F2AB-426A-4D5B-A1BB-2F30A914B883}">
+  <dimension ref="A1:C16"/>
+  <sheetViews>
+    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="50.7109375" customWidth="1"/>
+    <col min="2" max="3" width="15.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="2"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="2"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="2"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="2"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="2"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="2"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="2"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="2"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="2"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="2"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="2"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A13:C13"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DBFE07D-6F37-46A6-BAD9-AC9F73001E51}">
+  <dimension ref="A1:C16"/>
+  <sheetViews>
+    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="50.7109375" customWidth="1"/>
+    <col min="2" max="3" width="15.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A13:C13"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD9A0D6B-A634-407C-AD95-76C752B3D713}">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="50.7109375" customWidth="1"/>
+    <col min="2" max="3" width="15.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A7:C7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
03_Sprint_Backlogs.xlsx: Sprint #6 Daten aktualisiert. Vorherige Sprint-Backlogs aber noch nicht auf Stand.
</commit_message>
<xml_diff>
--- a/1. Projektplanung/03_Sprint_Backlogs.xlsx
+++ b/1. Projektplanung/03_Sprint_Backlogs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://thude0-my.sharepoint.com/personal/jecklu01_hs-ulm_de/Documents/5. Semester/Software Projekt/RaytRazor/1. Projektplanung/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="197" documentId="11_AD4DB114E441178AC67DF4622615E776693EDF11" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DDBF27A5-4643-488B-9C4F-9F2C570D61B7}"/>
+  <xr:revisionPtr revIDLastSave="445" documentId="11_AD4DB114E441178AC67DF4622615E776693EDF11" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F3B63915-7A1B-4393-826B-D80013A9680F}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="60">
   <si>
     <t>Aufgabe</t>
   </si>
@@ -101,33 +101,9 @@
     <t>medium</t>
   </si>
   <si>
-    <t>Übersicht über verschiedene Raytracing Arten verschaffen</t>
-  </si>
-  <si>
-    <t>Übersicht über math. Formeln für Raytracing verschaffen</t>
-  </si>
-  <si>
-    <t>Eigene Mathe-Bibliothek für Raytracing schreiben</t>
-  </si>
-  <si>
     <t>abgebrochen</t>
   </si>
   <si>
-    <t>GitHub Commit Layout definieren</t>
-  </si>
-  <si>
-    <t>GitHub Repository erstellen</t>
-  </si>
-  <si>
-    <t>Visionspräsentation erstellen und Präsentation abhalten</t>
-  </si>
-  <si>
-    <t>Team Zusammenstellung Hr. Lunde mitteilen</t>
-  </si>
-  <si>
-    <t>Mit .obj und .mtl Formaten vertraut machen</t>
-  </si>
-  <si>
     <t>Allgemeine Aufgaben</t>
   </si>
   <si>
@@ -135,6 +111,105 @@
   </si>
   <si>
     <t>Backend Aufgaben</t>
+  </si>
+  <si>
+    <t>3D-Preview -&gt; Objekte richtig darstellen.</t>
+  </si>
+  <si>
+    <t>3D-Preview -&gt; Objekte an Raytracer übergeben.</t>
+  </si>
+  <si>
+    <t>3D-Preview / Parser -&gt; Objekte dynamisch aus JSON laden.</t>
+  </si>
+  <si>
+    <t>Error-Handling -&gt; Logging via Logger-Klasse verbessern</t>
+  </si>
+  <si>
+    <t>Raytracing -&gt; Übergabe 3D-Preview verarbeiten können</t>
+  </si>
+  <si>
+    <t>Raytracing -&gt; Optimierungen implementieren</t>
+  </si>
+  <si>
+    <t>Raytracing -&gt; Bildexport ermöglichen</t>
+  </si>
+  <si>
+    <t>Main-Szene -&gt; Import einer Szene über Explorer aufruf</t>
+  </si>
+  <si>
+    <t>Main-Szene -&gt; Funktionalität Top-Bar Buttons impl.</t>
+  </si>
+  <si>
+    <t>Main-Szene -&gt; Schönere Darstellung Component Attrib.</t>
+  </si>
+  <si>
+    <t>Main-Szene -&gt; Schönere Darstellung Component Tree</t>
+  </si>
+  <si>
+    <t>Main-Szene -&gt; Funktionalität Component Tree</t>
+  </si>
+  <si>
+    <t>Main-Szene -&gt; Funktionalität Component Attributes</t>
+  </si>
+  <si>
+    <t>Allgemeine-Aufgaben</t>
+  </si>
+  <si>
+    <t>Lastenheft</t>
+  </si>
+  <si>
+    <t>Wiki-Page -&gt; Anleitung hinzufügen</t>
+  </si>
+  <si>
+    <t>Wiki-Page -&gt; Szenen-JSON Aufbau hinzufügen</t>
+  </si>
+  <si>
+    <t>Wiki-Page -&gt; Szenen-JSON Beispiel hinzufügen</t>
+  </si>
+  <si>
+    <t>Wiki-Page -&gt; UML Diagramm hinzufügen</t>
+  </si>
+  <si>
+    <t>Sprint-Backlogs -&gt; Einträge nachtragen</t>
+  </si>
+  <si>
+    <t>Product-Backlog -&gt; Einträge aktualisieren</t>
+  </si>
+  <si>
+    <t>Release-Präsentation -&gt; Management Ebene erstellen</t>
+  </si>
+  <si>
+    <t>Release-Präsentation -&gt; Technische Ebene erstellen</t>
+  </si>
+  <si>
+    <t>Raytracing -&gt; Übersicht über versch. Arten verschaffen</t>
+  </si>
+  <si>
+    <t>Raytracing -&gt; Übersicht über math. Formeln verschaffen</t>
+  </si>
+  <si>
+    <t>GitHub -&gt; Commit Layout definieren</t>
+  </si>
+  <si>
+    <t>GitHub -&gt; Repository erstellen</t>
+  </si>
+  <si>
+    <t>Visionspräsentation -&gt; Erstellen und abhalten</t>
+  </si>
+  <si>
+    <t>Management -&gt; Team-Composition an Management</t>
+  </si>
+  <si>
+    <t>Importer -&gt; Mit .obj/.mtl Formaten vertraut machen</t>
+  </si>
+  <si>
+    <t>Raytracing -&gt; Eigene Mathe-Bibliothek erstellen</t>
+  </si>
+  <si>
+    <t>Teams -&gt; Projekt-Team erstellen und Aufgaben planen</t>
+  </si>
+  <si>
+    <t>Meilenstein -&gt; Präsentation erstellen</t>
   </si>
 </sst>
 </file>
@@ -158,7 +233,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -195,8 +270,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -219,11 +300,59 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -233,6 +362,17 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -517,10 +657,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -542,137 +682,129 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>23</v>
+        <v>50</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="2"/>
+      <c r="C3" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>24</v>
+      <c r="A4" s="11" t="s">
+        <v>51</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="2"/>
+      <c r="C4" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>27</v>
+      <c r="A5" s="11" t="s">
+        <v>52</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="2"/>
+      <c r="C5" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>28</v>
+      <c r="A6" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="2"/>
+      <c r="C6" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>29</v>
+      <c r="A7" s="11" t="s">
+        <v>54</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="2"/>
+      <c r="C7" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>30</v>
+      <c r="A8" s="11" t="s">
+        <v>55</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="2"/>
+      <c r="C8" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>31</v>
+      <c r="A9" s="11" t="s">
+        <v>58</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="2"/>
+      <c r="C9" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="2"/>
+      <c r="A10" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="2"/>
+      <c r="A11" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
+      <c r="A12" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="2"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="2"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="2"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="2"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A11:C11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -680,121 +812,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F604C2F-B85D-43C9-892C-B1D90A990BEC}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="50.7109375" customWidth="1"/>
-    <col min="2" max="3" width="15.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="2"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="2"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="2"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="2"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="2"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="2"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="2"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="2"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="2"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="2"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="2"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="2"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="2"/>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A13:C13"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F033D8F3-60F5-4555-AEA9-6349E4C0E2BD}">
-  <dimension ref="A1:C16"/>
-  <sheetViews>
-    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C2"/>
+    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -816,76 +837,88 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="2"/>
+      <c r="A3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
-      <c r="B4" s="3"/>
+      <c r="B4" s="5"/>
       <c r="C4" s="2"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
-      <c r="B5" s="5"/>
+      <c r="B5" s="3"/>
       <c r="C5" s="2"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="2"/>
+      <c r="A6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="2"/>
+      <c r="A7" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
-      <c r="B8" s="4"/>
+      <c r="B8" s="3"/>
       <c r="C8" s="2"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
-      <c r="B9" s="4"/>
+      <c r="B9" s="5"/>
       <c r="C9" s="2"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
-      <c r="B10" s="4"/>
+      <c r="B10" s="5"/>
       <c r="C10" s="2"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
-      <c r="B11" s="3"/>
+      <c r="B11" s="5"/>
       <c r="C11" s="2"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
-      <c r="B12" s="5"/>
+      <c r="B12" s="4"/>
       <c r="C12" s="2"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
+      <c r="A13" s="2"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="2"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
-      <c r="B14" s="5"/>
+      <c r="B14" s="4"/>
       <c r="C14" s="2"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
-      <c r="B15" s="5"/>
+      <c r="B15" s="3"/>
       <c r="C15" s="2"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -893,21 +926,44 @@
       <c r="B16" s="5"/>
       <c r="C16" s="2"/>
     </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="2"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="2"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="2"/>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A17:C17"/>
     <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A13:C13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC71F2AB-426A-4D5B-A1BB-2F30A914B883}">
-  <dimension ref="A1:C16"/>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F033D8F3-60F5-4555-AEA9-6349E4C0E2BD}">
+  <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView topLeftCell="A6" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -929,76 +985,88 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="2"/>
+      <c r="A3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
-      <c r="B4" s="3"/>
+      <c r="B4" s="5"/>
       <c r="C4" s="2"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="2"/>
+      <c r="A5" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="2"/>
+      <c r="A6" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="9"/>
+      <c r="C6" s="10"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
-      <c r="B7" s="5"/>
+      <c r="B7" s="3"/>
       <c r="C7" s="2"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
-      <c r="B8" s="4"/>
+      <c r="B8" s="3"/>
       <c r="C8" s="2"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
-      <c r="B9" s="4"/>
+      <c r="B9" s="5"/>
       <c r="C9" s="2"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
-      <c r="B10" s="4"/>
+      <c r="B10" s="5"/>
       <c r="C10" s="2"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
-      <c r="B11" s="3"/>
+      <c r="B11" s="5"/>
       <c r="C11" s="2"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
-      <c r="B12" s="5"/>
+      <c r="B12" s="4"/>
       <c r="C12" s="2"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
+      <c r="A13" s="2"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="2"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
-      <c r="B14" s="5"/>
+      <c r="B14" s="4"/>
       <c r="C14" s="2"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
-      <c r="B15" s="5"/>
+      <c r="B15" s="3"/>
       <c r="C15" s="2"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -1006,21 +1074,44 @@
       <c r="B16" s="5"/>
       <c r="C16" s="2"/>
     </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="2"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="2"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="2"/>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A17:C17"/>
     <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A13:C13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DBFE07D-6F37-46A6-BAD9-AC9F73001E51}">
-  <dimension ref="A1:C16"/>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC71F2AB-426A-4D5B-A1BB-2F30A914B883}">
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="C3" sqref="A3:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1042,17 +1133,17 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>3</v>
+        <v>41</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>20</v>
@@ -1060,10 +1151,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>3</v>
+        <v>46</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>5</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>20</v>
@@ -1071,7 +1162,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>5</v>
@@ -1081,136 +1172,101 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>22</v>
-      </c>
+      <c r="A6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>22</v>
-      </c>
+      <c r="A7" s="2"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="2"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>20</v>
-      </c>
+      <c r="A8" s="2"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="2"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>20</v>
-      </c>
+      <c r="A9" s="2"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="2"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>20</v>
-      </c>
+      <c r="A10" s="2"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="2"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>20</v>
-      </c>
+      <c r="A11" s="2"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="2"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>20</v>
-      </c>
+      <c r="A12" s="2"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="2"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="2"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="2"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="2"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="2"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="2"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>22</v>
-      </c>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="2"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="2"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A17:C17"/>
     <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A13:C13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD9A0D6B-A634-407C-AD95-76C752B3D713}">
-  <dimension ref="A1:C10"/>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DBFE07D-6F37-46A6-BAD9-AC9F73001E51}">
+  <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0"/>
+    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:C5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1230,18 +1286,250 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="9"/>
+      <c r="C2" s="10"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="9"/>
+      <c r="C6" s="10"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="A2:C2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD9A0D6B-A634-407C-AD95-76C752B3D713}">
+  <dimension ref="A1:C29"/>
+  <sheetViews>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="50.7109375" customWidth="1"/>
+    <col min="2" max="3" width="15.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>5</v>
+        <v>41</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>20</v>
@@ -1249,7 +1537,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>5</v>
@@ -1260,7 +1548,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>5</v>
@@ -1271,59 +1559,265 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>13</v>
+        <v>44</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
+      <c r="A7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>5</v>
+        <v>46</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>5</v>
+        <v>47</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="2" t="s">
+      <c r="B29" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>22</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A21:C21"/>
     <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A7:C7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>